<commit_message>
change TRY analysis bounds and steps for FGI paper, and remove use of set_production_capacity from HP models for FGI
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_TAL_A_FGI_sugarcane.xlsx
+++ b/biorefineries/TAL/analyses/full/parameter_distributions/parameter-distributions_TAL_A_FGI_sugarcane.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\TAL\analyses\full\parameter_distributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E67A9FE-1E0C-436F-B847-9666D2C459F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B5BB13-351D-4C5F-839F-6742993A89CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,7 +671,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:I10"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>